<commit_message>
Relatório da primeira parte.
</commit_message>
<xml_diff>
--- a/TP/dados/Tentativa1.xlsx
+++ b/TP/dados/Tentativa1.xlsx
@@ -4,17 +4,24 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="15990" windowHeight="8940"/>
+    <workbookView windowWidth="19890" windowHeight="8940" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10">
+  <si>
+    <t>Naive</t>
+  </si>
+  <si>
+    <t>Naive-Borba</t>
+  </si>
   <si>
     <t>Tamanho</t>
   </si>
@@ -30,18 +37,27 @@
   <si>
     <t>Melhora %Tot</t>
   </si>
+  <si>
+    <t>O3</t>
+  </si>
+  <si>
+    <t>Borba</t>
+  </si>
+  <si>
+    <t>Melhora %Total</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -51,7 +67,83 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -65,53 +157,8 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -127,15 +174,21 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -149,21 +202,6 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -171,26 +209,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -203,13 +226,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -221,49 +292,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -293,7 +334,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -305,7 +352,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -317,73 +400,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -394,6 +417,41 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -417,17 +475,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -465,32 +512,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -499,153 +522,156 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -811,7 +837,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$27</c:f>
+              <c:f>Sheet1!$A$3:$A$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
@@ -898,87 +924,87 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$27</c:f>
+              <c:f>Sheet1!$B$3:$B$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>2342.43</c:v>
+                  <c:v>1552.15</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2388.09</c:v>
+                  <c:v>1562.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2055.72</c:v>
+                  <c:v>2217.85</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2030.39</c:v>
+                  <c:v>2220.23</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1984.17</c:v>
+                  <c:v>2134.43</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1377.07</c:v>
+                  <c:v>1993.82</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2013.97</c:v>
+                  <c:v>2192.21</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1921.26</c:v>
+                  <c:v>2108.58</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1761.43</c:v>
+                  <c:v>1681.53</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1872.84</c:v>
+                  <c:v>2061.26</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1888.68</c:v>
+                  <c:v>2079.43</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>902.815</c:v>
+                  <c:v>958.805</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1799.91</c:v>
+                  <c:v>2071.31</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1885.14</c:v>
+                  <c:v>2081.68</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1373.75</c:v>
+                  <c:v>1607.43</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1875.92</c:v>
+                  <c:v>2082.33</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1856.26</c:v>
+                  <c:v>2065.68</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1866.12</c:v>
+                  <c:v>2079.83</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1730.83</c:v>
+                  <c:v>1938.44</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1872.94</c:v>
+                  <c:v>2091.01</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>848.425</c:v>
+                  <c:v>947.903</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1587.36</c:v>
+                  <c:v>2047.79</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>888.47</c:v>
+                  <c:v>957.56</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1576.14</c:v>
+                  <c:v>2046.49</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>846.02</c:v>
+                  <c:v>961.095</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1595.16</c:v>
+                  <c:v>2047.58</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1013,7 +1039,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$27</c:f>
+              <c:f>Sheet1!$A$3:$A$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
@@ -1100,87 +1126,87 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$27</c:f>
+              <c:f>Sheet1!$F$3:$F$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>2415.13</c:v>
+                  <c:v>1546.86</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2398.95</c:v>
+                  <c:v>1549.86</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2080.79</c:v>
+                  <c:v>2214.91</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2034.7</c:v>
+                  <c:v>2216.66</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2040.15</c:v>
+                  <c:v>2192.81</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1897.92</c:v>
+                  <c:v>1982</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1986.65</c:v>
+                  <c:v>2193.86</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1920.99</c:v>
+                  <c:v>2108.68</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1803.59</c:v>
+                  <c:v>1999.47</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1841.97</c:v>
+                  <c:v>2097.43</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1914.21</c:v>
+                  <c:v>2079.59</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>876.84</c:v>
+                  <c:v>983.56</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1904</c:v>
+                  <c:v>2072.44</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1904.92</c:v>
+                  <c:v>2078.3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1566.93</c:v>
+                  <c:v>1600.41</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1891.99</c:v>
+                  <c:v>2078.89</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1744.27</c:v>
+                  <c:v>2073.94</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1876.08</c:v>
+                  <c:v>2088.21</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1595.34</c:v>
+                  <c:v>1950.63</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1884.98</c:v>
+                  <c:v>2091.42</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>880.496</c:v>
+                  <c:v>951.529</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1604.08</c:v>
+                  <c:v>2065.19</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>903.644</c:v>
+                  <c:v>955.776</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1595.77</c:v>
+                  <c:v>2067.85</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>838.952</c:v>
+                  <c:v>963.38</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1593.23</c:v>
+                  <c:v>2068.21</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1496,7 +1522,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$27</c:f>
+              <c:f>Sheet1!$A$3:$A$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
@@ -1583,87 +1609,87 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$27</c:f>
+              <c:f>Sheet1!$C$3:$C$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>12.2</c:v>
+                  <c:v>8.08</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.44</c:v>
+                  <c:v>8.14</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.71</c:v>
+                  <c:v>11.55</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10.57</c:v>
+                  <c:v>11.56</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10.33</c:v>
+                  <c:v>11.12</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.17</c:v>
+                  <c:v>10.38</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10.49</c:v>
+                  <c:v>11.42</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10.01</c:v>
+                  <c:v>10.98</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.17</c:v>
+                  <c:v>8.76</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.75</c:v>
+                  <c:v>10.74</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9.84</c:v>
+                  <c:v>10.83</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.7</c:v>
+                  <c:v>4.99</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>9.37</c:v>
+                  <c:v>10.79</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>9.82</c:v>
+                  <c:v>10.84</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7.15</c:v>
+                  <c:v>8.37</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9.77</c:v>
+                  <c:v>10.85</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>9.67</c:v>
+                  <c:v>10.76</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9.72</c:v>
+                  <c:v>10.83</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9.01</c:v>
+                  <c:v>10.1</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>9.75</c:v>
+                  <c:v>10.89</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4.42</c:v>
+                  <c:v>4.94</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>8.27</c:v>
+                  <c:v>10.67</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>4.63</c:v>
+                  <c:v>4.99</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>8.21</c:v>
+                  <c:v>10.66</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>4.41</c:v>
+                  <c:v>5.01</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>8.31</c:v>
+                  <c:v>10.66</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1695,7 +1721,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$27</c:f>
+              <c:f>Sheet1!$A$3:$A$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
@@ -1782,87 +1808,87 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$2:$G$27</c:f>
+              <c:f>Sheet1!$G$3:$G$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>12.58</c:v>
+                  <c:v>8.06</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.49</c:v>
+                  <c:v>8.07</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.84</c:v>
+                  <c:v>11.54</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10.6</c:v>
+                  <c:v>11.55</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10.63</c:v>
+                  <c:v>11.42</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.88</c:v>
+                  <c:v>10.32</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10.35</c:v>
+                  <c:v>11.43</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10.01</c:v>
+                  <c:v>10.98</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.39</c:v>
+                  <c:v>10.41</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.59</c:v>
+                  <c:v>10.92</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9.97</c:v>
+                  <c:v>10.83</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.57</c:v>
+                  <c:v>5.12</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>9.92</c:v>
+                  <c:v>10.79</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>9.92</c:v>
+                  <c:v>10.82</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>8.16</c:v>
+                  <c:v>8.34</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9.85</c:v>
+                  <c:v>10.83</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>9.08</c:v>
+                  <c:v>10.8</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9.77</c:v>
+                  <c:v>10.88</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>8.31</c:v>
+                  <c:v>10.16</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>9.82</c:v>
+                  <c:v>10.89</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4.59</c:v>
+                  <c:v>4.96</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>8.35</c:v>
+                  <c:v>10.76</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>4.71</c:v>
+                  <c:v>4.98</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>8.31</c:v>
+                  <c:v>10.77</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>4.37</c:v>
+                  <c:v>5.02</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>8.3</c:v>
+                  <c:v>10.77</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2166,7 +2192,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$27</c:f>
+              <c:f>Sheet1!$A$3:$A$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
@@ -2253,87 +2279,87 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$J$2:$J$27</c:f>
+              <c:f>Sheet1!$J$3:$J$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>0.380000000000001</c:v>
+                  <c:v>-0.0199999999999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0500000000000007</c:v>
+                  <c:v>-0.0700000000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.129999999999999</c:v>
+                  <c:v>-0.0100000000000016</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0299999999999994</c:v>
+                  <c:v>-0.00999999999999979</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.300000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.71</c:v>
+                  <c:v>-0.0600000000000005</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.140000000000001</c:v>
+                  <c:v>0.00999999999999979</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.220000000000001</c:v>
+                  <c:v>1.65</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.16</c:v>
+                  <c:v>0.18</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.130000000000001</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.13</c:v>
+                  <c:v>0.13</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.550000000000001</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.0999999999999996</c:v>
+                  <c:v>-0.0199999999999996</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.01</c:v>
+                  <c:v>-0.0299999999999994</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.0800000000000001</c:v>
+                  <c:v>-0.0199999999999996</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-0.59</c:v>
+                  <c:v>0.0400000000000009</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.0499999999999989</c:v>
+                  <c:v>0.0500000000000007</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-0.699999999999999</c:v>
+                  <c:v>0.0600000000000005</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.0700000000000003</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.17</c:v>
+                  <c:v>0.0199999999999996</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.0800000000000001</c:v>
+                  <c:v>0.0899999999999999</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.0800000000000001</c:v>
+                  <c:v>-0.00999999999999979</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.0999999999999996</c:v>
+                  <c:v>0.109999999999999</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-0.04</c:v>
+                  <c:v>0.00999999999999979</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>-0.00999999999999979</c:v>
+                  <c:v>0.109999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2511,6 +2537,417 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" horzOverflow="overflow" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$A$3:$A$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>127</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>129</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>191</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>229</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>255</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>257</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>319</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>321</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>417</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>479</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>511</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>639</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>640</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>767</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>768</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>769</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$J$3:$J$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>-0.100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.0899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.23</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.110000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.0899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.220000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.109999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.0899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.0399999999999991</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.0899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-0.100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-0.19</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-0.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-0.0800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.960000000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-0.100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-0.119999999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-0.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-0.0800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-0.04</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-0.0599999999999996</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.0399999999999991</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-0.0499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.0199999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="183660181"/>
+        <c:axId val="277200910"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="183660181"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" horzOverflow="overflow" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="277200910"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickMarkSkip val="1"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="277200910"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" horzOverflow="overflow" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="183660181"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" horzOverflow="overflow" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr lang="en-US" sz="1000" kern="1200">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:latin typeface="+mn-lt"/>
+          <a:ea typeface="+mn-ea"/>
+          <a:cs typeface="+mn-cs"/>
+        </a:defRPr>
+      </a:pPr>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins r="0.7" b="0.75" l="0.7" footer="0.3" header="0.3" t="0.75"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2631,6 +3068,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -4153,19 +4630,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>635</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>381635</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
@@ -4174,8 +5154,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="635" y="4857750"/>
-        <a:ext cx="4572000" cy="2743200"/>
+        <a:off x="9525" y="5019675"/>
+        <a:ext cx="5743575" cy="2743200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4187,16 +5167,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>372110</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>704850</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4204,8 +5184,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5353050" y="4829175"/>
-        <a:ext cx="5029200" cy="2743200"/>
+        <a:off x="6239510" y="4943475"/>
+        <a:ext cx="6162040" cy="2743200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4219,13 +5199,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>696595</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>286385</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>67</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
@@ -4234,7 +5214,7 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="696595" y="8058150"/>
+        <a:off x="696595" y="8220075"/>
         <a:ext cx="6295390" cy="2743200"/>
       </xdr:xfrm>
       <a:graphic>
@@ -4246,6 +5226,110 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="152400" y="4838700"/>
+        <a:ext cx="6553200" cy="2743200"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:C28" headerRowCount="0" totalsRowShown="0">
+  <tableColumns count="3">
+    <tableColumn id="1" name="Column1"/>
+    <tableColumn id="2" name="Column2"/>
+    <tableColumn id="3" name="Column3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="E2:G28">
+  <autoFilter ref="E2:G28"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Tamanho" totalsRowLabel="Total"/>
+    <tableColumn id="2" name="MFlops"/>
+    <tableColumn id="3" name="% Total" totalsRowFunction="sum"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="I2:J28" totalsRowShown="0">
+  <autoFilter ref="I2:J28"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Melhora MFlops"/>
+    <tableColumn id="2" name="Melhora %Tot"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A2:C28" totalsRowShown="0">
+  <autoFilter ref="A2:C28"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Tamanho"/>
+    <tableColumn id="2" name="MFlops"/>
+    <tableColumn id="3" name="% Total"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="E2:G28" totalsRowShown="0">
+  <autoFilter ref="E2:G28"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Tamanho"/>
+    <tableColumn id="2" name="MFlops"/>
+    <tableColumn id="3" name="% Total"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="I2:J28" totalsRowShown="0">
+  <autoFilter ref="I2:J28"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Melhora MFlops"/>
+    <tableColumn id="2" name="Melhora %Total"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4507,774 +5591,1580 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="J60" sqref="J60"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75"/>
   <cols>
     <col min="9" max="9" width="13.6" customWidth="1"/>
+    <col min="10" max="10" width="13.8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
+    <row r="1" spans="2:6">
       <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
         <v>0</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2">
-        <v>31</v>
-      </c>
-      <c r="B2">
-        <v>2342.43</v>
-      </c>
-      <c r="C2">
-        <v>12.2</v>
-      </c>
-      <c r="E2">
-        <v>31</v>
-      </c>
-      <c r="F2">
-        <v>2415.13</v>
-      </c>
-      <c r="G2">
-        <v>12.58</v>
-      </c>
-      <c r="I2">
-        <f>F2/B2</f>
-        <v>1.03103614622422</v>
-      </c>
-      <c r="J2">
-        <f>G2-C2</f>
-        <v>0.380000000000001</v>
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3">
-        <v>2388.09</v>
+        <v>1552.15</v>
       </c>
       <c r="C3">
-        <v>12.44</v>
+        <v>8.08</v>
       </c>
       <c r="E3">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F3">
-        <v>2398.95</v>
+        <v>1546.86</v>
       </c>
       <c r="G3">
-        <v>12.49</v>
+        <v>8.06</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I27" si="0">F3/B3</f>
-        <v>1.00454756730274</v>
+        <f>F3/B3</f>
+        <v>0.996591824243791</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J27" si="1">G3-C3</f>
-        <v>0.0500000000000007</v>
+        <f>G3-C3</f>
+        <v>-0.0199999999999996</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4">
-        <v>96</v>
+        <v>32</v>
       </c>
       <c r="B4">
-        <v>2055.72</v>
+        <v>1562.75</v>
       </c>
       <c r="C4">
-        <v>10.71</v>
+        <v>8.14</v>
       </c>
       <c r="E4">
-        <v>96</v>
+        <v>32</v>
       </c>
       <c r="F4">
-        <v>2080.79</v>
+        <v>1549.86</v>
       </c>
       <c r="G4">
-        <v>10.84</v>
+        <v>8.07</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
-        <v>1.01219524059697</v>
+        <f t="shared" ref="I4:I28" si="0">F4/B4</f>
+        <v>0.991751719724844</v>
       </c>
       <c r="J4">
-        <f t="shared" si="1"/>
-        <v>0.129999999999999</v>
+        <f t="shared" ref="J4:J28" si="1">G4-C4</f>
+        <v>-0.0700000000000003</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B5">
-        <v>2030.39</v>
+        <v>2217.85</v>
       </c>
       <c r="C5">
-        <v>10.57</v>
+        <v>11.55</v>
       </c>
       <c r="E5">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F5">
-        <v>2034.7</v>
+        <v>2214.91</v>
       </c>
       <c r="G5">
-        <v>10.6</v>
+        <v>11.54</v>
       </c>
       <c r="I5">
         <f t="shared" si="0"/>
-        <v>1.00212274489138</v>
+        <v>0.998674391865996</v>
       </c>
       <c r="J5">
         <f t="shared" si="1"/>
-        <v>0.0299999999999994</v>
+        <v>-0.0100000000000016</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6">
-        <v>127</v>
+        <v>97</v>
       </c>
       <c r="B6">
-        <v>1984.17</v>
+        <v>2220.23</v>
       </c>
       <c r="C6">
-        <v>10.33</v>
+        <v>11.56</v>
       </c>
       <c r="E6">
-        <v>127</v>
+        <v>97</v>
       </c>
       <c r="F6">
-        <v>2040.15</v>
+        <v>2216.66</v>
       </c>
       <c r="G6">
-        <v>10.63</v>
+        <v>11.55</v>
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>1.02821330833548</v>
+        <v>0.998392058480428</v>
       </c>
       <c r="J6">
         <f t="shared" si="1"/>
-        <v>0.300000000000001</v>
+        <v>-0.00999999999999979</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B7">
-        <v>1377.07</v>
+        <v>2134.43</v>
       </c>
       <c r="C7">
-        <v>7.17</v>
+        <v>11.12</v>
       </c>
       <c r="E7">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F7">
-        <v>1897.92</v>
+        <v>2192.81</v>
       </c>
       <c r="G7">
-        <v>9.88</v>
+        <v>11.42</v>
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>1.37823059103749</v>
+        <v>1.02735156458633</v>
       </c>
       <c r="J7">
         <f t="shared" si="1"/>
-        <v>2.71</v>
+        <v>0.300000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B8">
-        <v>2013.97</v>
+        <v>1993.82</v>
       </c>
       <c r="C8">
-        <v>10.49</v>
+        <v>10.38</v>
       </c>
       <c r="E8">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F8">
-        <v>1986.65</v>
+        <v>1982</v>
       </c>
       <c r="G8">
-        <v>10.35</v>
+        <v>10.32</v>
       </c>
       <c r="I8">
         <f t="shared" si="0"/>
-        <v>0.986434753248559</v>
+        <v>0.994071681495822</v>
       </c>
       <c r="J8">
         <f t="shared" si="1"/>
-        <v>-0.140000000000001</v>
+        <v>-0.0600000000000005</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9">
-        <v>191</v>
+        <v>129</v>
       </c>
       <c r="B9">
-        <v>1921.26</v>
+        <v>2192.21</v>
       </c>
       <c r="C9">
-        <v>10.01</v>
+        <v>11.42</v>
       </c>
       <c r="E9">
-        <v>191</v>
+        <v>129</v>
       </c>
       <c r="F9">
-        <v>1920.99</v>
+        <v>2193.86</v>
       </c>
       <c r="G9">
-        <v>10.01</v>
+        <v>11.43</v>
       </c>
       <c r="I9">
         <f t="shared" si="0"/>
-        <v>0.999859467224634</v>
+        <v>1.00075266511876</v>
       </c>
       <c r="J9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.00999999999999979</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B10">
-        <v>1761.43</v>
+        <v>2108.58</v>
       </c>
       <c r="C10">
-        <v>9.17</v>
+        <v>10.98</v>
       </c>
       <c r="E10">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F10">
-        <v>1803.59</v>
+        <v>2108.68</v>
       </c>
       <c r="G10">
-        <v>9.39</v>
+        <v>10.98</v>
       </c>
       <c r="I10">
         <f t="shared" si="0"/>
-        <v>1.02393509818727</v>
+        <v>1.00004742528147</v>
       </c>
       <c r="J10">
         <f t="shared" si="1"/>
-        <v>0.220000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11">
-        <v>229</v>
+        <v>192</v>
       </c>
       <c r="B11">
-        <v>1872.84</v>
+        <v>1681.53</v>
       </c>
       <c r="C11">
-        <v>9.75</v>
+        <v>8.76</v>
       </c>
       <c r="E11">
-        <v>229</v>
+        <v>192</v>
       </c>
       <c r="F11">
-        <v>1841.97</v>
+        <v>1999.47</v>
       </c>
       <c r="G11">
-        <v>9.59</v>
+        <v>10.41</v>
       </c>
       <c r="I11">
         <f t="shared" si="0"/>
-        <v>0.98351701159736</v>
+        <v>1.18907780414266</v>
       </c>
       <c r="J11">
         <f t="shared" si="1"/>
-        <v>-0.16</v>
+        <v>1.65</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12">
-        <v>255</v>
+        <v>229</v>
       </c>
       <c r="B12">
-        <v>1888.68</v>
+        <v>2061.26</v>
       </c>
       <c r="C12">
-        <v>9.84</v>
+        <v>10.74</v>
       </c>
       <c r="E12">
-        <v>255</v>
+        <v>229</v>
       </c>
       <c r="F12">
-        <v>1914.21</v>
+        <v>2097.43</v>
       </c>
       <c r="G12">
-        <v>9.97</v>
+        <v>10.92</v>
       </c>
       <c r="I12">
         <f t="shared" si="0"/>
-        <v>1.01351737721583</v>
+        <v>1.01754751947838</v>
       </c>
       <c r="J12">
         <f t="shared" si="1"/>
-        <v>0.130000000000001</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B13">
-        <v>902.815</v>
+        <v>2079.43</v>
       </c>
       <c r="C13">
-        <v>4.7</v>
+        <v>10.83</v>
       </c>
       <c r="E13">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F13">
-        <v>876.84</v>
+        <v>2079.59</v>
       </c>
       <c r="G13">
-        <v>4.57</v>
+        <v>10.83</v>
       </c>
       <c r="I13">
         <f t="shared" si="0"/>
-        <v>0.971228878563161</v>
+        <v>1.00007694416258</v>
       </c>
       <c r="J13">
         <f t="shared" si="1"/>
-        <v>-0.13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B14">
-        <v>1799.91</v>
+        <v>958.805</v>
       </c>
       <c r="C14">
-        <v>9.37</v>
+        <v>4.99</v>
       </c>
       <c r="E14">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F14">
-        <v>1904</v>
+        <v>983.56</v>
       </c>
       <c r="G14">
-        <v>9.92</v>
+        <v>5.12</v>
       </c>
       <c r="I14">
         <f t="shared" si="0"/>
-        <v>1.05783066931124</v>
+        <v>1.02581859710786</v>
       </c>
       <c r="J14">
         <f t="shared" si="1"/>
-        <v>0.550000000000001</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15">
-        <v>319</v>
+        <v>257</v>
       </c>
       <c r="B15">
-        <v>1885.14</v>
+        <v>2071.31</v>
       </c>
       <c r="C15">
-        <v>9.82</v>
+        <v>10.79</v>
       </c>
       <c r="E15">
-        <v>319</v>
+        <v>257</v>
       </c>
       <c r="F15">
-        <v>1904.92</v>
+        <v>2072.44</v>
       </c>
       <c r="G15">
-        <v>9.92</v>
+        <v>10.79</v>
       </c>
       <c r="I15">
         <f t="shared" si="0"/>
-        <v>1.01049258940981</v>
+        <v>1.00054554846933</v>
       </c>
       <c r="J15">
         <f t="shared" si="1"/>
-        <v>0.0999999999999996</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B16">
-        <v>1373.75</v>
+        <v>2081.68</v>
       </c>
       <c r="C16">
-        <v>7.15</v>
+        <v>10.84</v>
       </c>
       <c r="E16">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F16">
-        <v>1566.93</v>
+        <v>2078.3</v>
       </c>
       <c r="G16">
-        <v>8.16</v>
+        <v>10.82</v>
       </c>
       <c r="I16">
         <f t="shared" si="0"/>
-        <v>1.14062238398544</v>
+        <v>0.99837631144076</v>
       </c>
       <c r="J16">
         <f t="shared" si="1"/>
-        <v>1.01</v>
+        <v>-0.0199999999999996</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B17">
-        <v>1875.92</v>
+        <v>1607.43</v>
       </c>
       <c r="C17">
-        <v>9.77</v>
+        <v>8.37</v>
       </c>
       <c r="E17">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F17">
-        <v>1891.99</v>
+        <v>1600.41</v>
       </c>
       <c r="G17">
-        <v>9.85</v>
+        <v>8.34</v>
       </c>
       <c r="I17">
         <f t="shared" si="0"/>
-        <v>1.00856646338863</v>
+        <v>0.995632780276591</v>
       </c>
       <c r="J17">
         <f t="shared" si="1"/>
-        <v>0.0800000000000001</v>
+        <v>-0.0299999999999994</v>
       </c>
     </row>
     <row r="18" spans="1:10">
       <c r="A18">
-        <v>417</v>
+        <v>321</v>
       </c>
       <c r="B18">
-        <v>1856.26</v>
+        <v>2082.33</v>
       </c>
       <c r="C18">
-        <v>9.67</v>
+        <v>10.85</v>
       </c>
       <c r="E18">
-        <v>417</v>
+        <v>321</v>
       </c>
       <c r="F18">
-        <v>1744.27</v>
+        <v>2078.89</v>
       </c>
       <c r="G18">
-        <v>9.08</v>
+        <v>10.83</v>
       </c>
       <c r="I18">
         <f t="shared" si="0"/>
-        <v>0.939669011884111</v>
+        <v>0.998348004398918</v>
       </c>
       <c r="J18">
         <f t="shared" si="1"/>
-        <v>-0.59</v>
+        <v>-0.0199999999999996</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19">
-        <v>479</v>
+        <v>417</v>
       </c>
       <c r="B19">
-        <v>1866.12</v>
+        <v>2065.68</v>
       </c>
       <c r="C19">
-        <v>9.72</v>
+        <v>10.76</v>
       </c>
       <c r="E19">
-        <v>479</v>
+        <v>417</v>
       </c>
       <c r="F19">
-        <v>1876.08</v>
+        <v>2073.94</v>
       </c>
       <c r="G19">
-        <v>9.77</v>
+        <v>10.8</v>
       </c>
       <c r="I19">
         <f t="shared" si="0"/>
-        <v>1.00533727734551</v>
+        <v>1.00399868324232</v>
       </c>
       <c r="J19">
         <f t="shared" si="1"/>
-        <v>0.0499999999999989</v>
+        <v>0.0400000000000009</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B20">
-        <v>1730.83</v>
+        <v>2079.83</v>
       </c>
       <c r="C20">
-        <v>9.01</v>
+        <v>10.83</v>
       </c>
       <c r="E20">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="F20">
-        <v>1595.34</v>
+        <v>2088.21</v>
       </c>
       <c r="G20">
-        <v>8.31</v>
+        <v>10.88</v>
       </c>
       <c r="I20">
         <f t="shared" si="0"/>
-        <v>0.921719637399398</v>
+        <v>1.00402917546146</v>
       </c>
       <c r="J20">
         <f t="shared" si="1"/>
-        <v>-0.699999999999999</v>
+        <v>0.0500000000000007</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21">
-        <v>511</v>
+        <v>480</v>
       </c>
       <c r="B21">
-        <v>1872.94</v>
+        <v>1938.44</v>
       </c>
       <c r="C21">
-        <v>9.75</v>
+        <v>10.1</v>
       </c>
       <c r="E21">
-        <v>511</v>
+        <v>480</v>
       </c>
       <c r="F21">
-        <v>1884.98</v>
+        <v>1950.63</v>
       </c>
       <c r="G21">
-        <v>9.82</v>
+        <v>10.16</v>
       </c>
       <c r="I21">
         <f t="shared" si="0"/>
-        <v>1.00642839599774</v>
+        <v>1.0062885619364</v>
       </c>
       <c r="J21">
         <f t="shared" si="1"/>
-        <v>0.0700000000000003</v>
+        <v>0.0600000000000005</v>
       </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B22">
-        <v>848.425</v>
+        <v>2091.01</v>
       </c>
       <c r="C22">
-        <v>4.42</v>
+        <v>10.89</v>
       </c>
       <c r="E22">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="F22">
-        <v>880.496</v>
+        <v>2091.42</v>
       </c>
       <c r="G22">
-        <v>4.59</v>
+        <v>10.89</v>
       </c>
       <c r="I22">
         <f t="shared" si="0"/>
-        <v>1.03780063058019</v>
+        <v>1.00019607749365</v>
       </c>
       <c r="J22">
         <f t="shared" si="1"/>
-        <v>0.17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:10">
       <c r="A23">
-        <v>639</v>
+        <v>512</v>
       </c>
       <c r="B23">
-        <v>1587.36</v>
+        <v>947.903</v>
       </c>
       <c r="C23">
-        <v>8.27</v>
+        <v>4.94</v>
       </c>
       <c r="E23">
-        <v>639</v>
+        <v>512</v>
       </c>
       <c r="F23">
-        <v>1604.08</v>
+        <v>951.529</v>
       </c>
       <c r="G23">
-        <v>8.35</v>
+        <v>4.96</v>
       </c>
       <c r="I23">
         <f t="shared" si="0"/>
-        <v>1.01053321237778</v>
+        <v>1.00382528592061</v>
       </c>
       <c r="J23">
         <f t="shared" si="1"/>
-        <v>0.0800000000000001</v>
+        <v>0.0199999999999996</v>
       </c>
     </row>
     <row r="24" spans="1:10">
       <c r="A24">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B24">
-        <v>888.47</v>
+        <v>2047.79</v>
       </c>
       <c r="C24">
-        <v>4.63</v>
+        <v>10.67</v>
       </c>
       <c r="E24">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="F24">
-        <v>903.644</v>
+        <v>2065.19</v>
       </c>
       <c r="G24">
-        <v>4.71</v>
+        <v>10.76</v>
       </c>
       <c r="I24">
         <f t="shared" si="0"/>
-        <v>1.01707879838374</v>
+        <v>1.00849696502083</v>
       </c>
       <c r="J24">
         <f t="shared" si="1"/>
-        <v>0.0800000000000001</v>
+        <v>0.0899999999999999</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25">
-        <v>767</v>
+        <v>640</v>
       </c>
       <c r="B25">
-        <v>1576.14</v>
+        <v>957.56</v>
       </c>
       <c r="C25">
-        <v>8.21</v>
+        <v>4.99</v>
       </c>
       <c r="E25">
-        <v>767</v>
+        <v>640</v>
       </c>
       <c r="F25">
-        <v>1595.77</v>
+        <v>955.776</v>
       </c>
       <c r="G25">
-        <v>8.31</v>
+        <v>4.98</v>
       </c>
       <c r="I25">
         <f t="shared" si="0"/>
-        <v>1.01245447739414</v>
+        <v>0.998136931367225</v>
       </c>
       <c r="J25">
         <f t="shared" si="1"/>
-        <v>0.0999999999999996</v>
+        <v>-0.00999999999999979</v>
       </c>
     </row>
     <row r="26" spans="1:10">
       <c r="A26">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="B26">
-        <v>846.02</v>
+        <v>2046.49</v>
       </c>
       <c r="C26">
-        <v>4.41</v>
+        <v>10.66</v>
       </c>
       <c r="E26">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="F26">
-        <v>838.952</v>
+        <v>2067.85</v>
       </c>
       <c r="G26">
-        <v>4.37</v>
+        <v>10.77</v>
       </c>
       <c r="I26">
         <f t="shared" si="0"/>
-        <v>0.991645587574762</v>
+        <v>1.01043738303143</v>
       </c>
       <c r="J26">
         <f t="shared" si="1"/>
-        <v>-0.04</v>
+        <v>0.109999999999999</v>
       </c>
     </row>
     <row r="27" spans="1:10">
       <c r="A27">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="B27">
-        <v>1595.16</v>
+        <v>961.095</v>
       </c>
       <c r="C27">
-        <v>8.31</v>
+        <v>5.01</v>
       </c>
       <c r="E27">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="F27">
-        <v>1593.23</v>
+        <v>963.38</v>
       </c>
       <c r="G27">
-        <v>8.3</v>
+        <v>5.02</v>
       </c>
       <c r="I27">
         <f t="shared" si="0"/>
-        <v>0.998790090022317</v>
+        <v>1.00237749650139</v>
       </c>
       <c r="J27">
         <f t="shared" si="1"/>
-        <v>-0.00999999999999979</v>
+        <v>0.00999999999999979</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28">
+        <v>769</v>
+      </c>
+      <c r="B28">
+        <v>2047.58</v>
+      </c>
+      <c r="C28">
+        <v>10.66</v>
+      </c>
+      <c r="E28">
+        <v>769</v>
+      </c>
+      <c r="F28">
+        <v>2068.21</v>
+      </c>
+      <c r="G28">
+        <v>10.77</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="0"/>
+        <v>1.01007530841286</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="1"/>
+        <v>0.109999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
+  <drawing r:id="rId1"/>
+  <tableParts count="3">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:J28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="9" max="9" width="17.4" customWidth="1"/>
+    <col min="10" max="10" width="14.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6">
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3">
+        <v>31</v>
+      </c>
+      <c r="B3">
+        <v>2121.44</v>
+      </c>
+      <c r="C3">
+        <v>11.05</v>
+      </c>
+      <c r="E3">
+        <v>31</v>
+      </c>
+      <c r="F3">
+        <v>2102.35</v>
+      </c>
+      <c r="G3">
+        <v>10.95</v>
+      </c>
+      <c r="I3">
+        <f>F3/B3</f>
+        <v>0.991001395278679</v>
+      </c>
+      <c r="J3">
+        <f>G3-C3</f>
+        <v>-0.100000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4">
+        <v>32</v>
+      </c>
+      <c r="B4">
+        <v>2122.5</v>
+      </c>
+      <c r="C4">
+        <v>11.05</v>
+      </c>
+      <c r="E4">
+        <v>32</v>
+      </c>
+      <c r="F4">
+        <v>2103.67</v>
+      </c>
+      <c r="G4">
+        <v>10.96</v>
+      </c>
+      <c r="I4">
+        <f t="shared" ref="I4:I28" si="0">F4/B4</f>
+        <v>0.991128386336867</v>
+      </c>
+      <c r="J4">
+        <f t="shared" ref="J4:J28" si="1">G4-C4</f>
+        <v>-0.0899999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5">
+        <v>96</v>
+      </c>
+      <c r="B5">
+        <v>2030.55</v>
+      </c>
+      <c r="C5">
+        <v>10.58</v>
+      </c>
+      <c r="E5">
+        <v>96</v>
+      </c>
+      <c r="F5">
+        <v>2075.33</v>
+      </c>
+      <c r="G5">
+        <v>10.81</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>1.02205313831228</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="1"/>
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6">
+        <v>97</v>
+      </c>
+      <c r="B6">
+        <v>2426.21</v>
+      </c>
+      <c r="C6">
+        <v>12.64</v>
+      </c>
+      <c r="E6">
+        <v>97</v>
+      </c>
+      <c r="F6">
+        <v>2406.62</v>
+      </c>
+      <c r="G6">
+        <v>12.53</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>0.991925678321332</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="1"/>
+        <v>-0.110000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7">
+        <v>127</v>
+      </c>
+      <c r="B7">
+        <v>2341.49</v>
+      </c>
+      <c r="C7">
+        <v>12.2</v>
+      </c>
+      <c r="E7">
+        <v>127</v>
+      </c>
+      <c r="F7">
+        <v>2324.23</v>
+      </c>
+      <c r="G7">
+        <v>12.11</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>0.992628625362483</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="1"/>
+        <v>-0.0899999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8">
+        <v>128</v>
+      </c>
+      <c r="B8">
+        <v>2142.08</v>
+      </c>
+      <c r="C8">
+        <v>11.16</v>
+      </c>
+      <c r="E8">
+        <v>128</v>
+      </c>
+      <c r="F8">
+        <v>2100.46</v>
+      </c>
+      <c r="G8">
+        <v>10.94</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>0.980570286824022</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="1"/>
+        <v>-0.220000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9">
+        <v>129</v>
+      </c>
+      <c r="B9">
+        <v>2341.52</v>
+      </c>
+      <c r="C9">
+        <v>12.2</v>
+      </c>
+      <c r="E9">
+        <v>129</v>
+      </c>
+      <c r="F9">
+        <v>2320.56</v>
+      </c>
+      <c r="G9">
+        <v>12.09</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>0.99104854966005</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="1"/>
+        <v>-0.109999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10">
+        <v>191</v>
+      </c>
+      <c r="B10">
+        <v>2161.54</v>
+      </c>
+      <c r="C10">
+        <v>11.26</v>
+      </c>
+      <c r="E10">
+        <v>191</v>
+      </c>
+      <c r="F10">
+        <v>2145.4</v>
+      </c>
+      <c r="G10">
+        <v>11.17</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>0.992533101399928</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="1"/>
+        <v>-0.0899999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11">
+        <v>192</v>
+      </c>
+      <c r="B11">
+        <v>2067.92</v>
+      </c>
+      <c r="C11">
+        <v>10.77</v>
+      </c>
+      <c r="E11">
+        <v>192</v>
+      </c>
+      <c r="F11">
+        <v>2061.06</v>
+      </c>
+      <c r="G11">
+        <v>10.73</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>0.996682656969322</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="1"/>
+        <v>-0.0399999999999991</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12">
+        <v>229</v>
+      </c>
+      <c r="B12">
+        <v>2143.01</v>
+      </c>
+      <c r="C12">
+        <v>11.16</v>
+      </c>
+      <c r="E12">
+        <v>229</v>
+      </c>
+      <c r="F12">
+        <v>2124.49</v>
+      </c>
+      <c r="G12">
+        <v>11.07</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>0.991357949799581</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="1"/>
+        <v>-0.0899999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13">
+        <v>255</v>
+      </c>
+      <c r="B13">
+        <v>2139.14</v>
+      </c>
+      <c r="C13">
+        <v>11.14</v>
+      </c>
+      <c r="E13">
+        <v>255</v>
+      </c>
+      <c r="F13">
+        <v>2120.13</v>
+      </c>
+      <c r="G13">
+        <v>11.04</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>0.991113251119609</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="1"/>
+        <v>-0.100000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14">
+        <v>256</v>
+      </c>
+      <c r="B14">
+        <v>996.283</v>
+      </c>
+      <c r="C14">
+        <v>5.19</v>
+      </c>
+      <c r="E14">
+        <v>256</v>
+      </c>
+      <c r="F14">
+        <v>959.91</v>
+      </c>
+      <c r="G14">
+        <v>5</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>0.963491297151512</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="1"/>
+        <v>-0.19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15">
+        <v>257</v>
+      </c>
+      <c r="B15">
+        <v>2140.66</v>
+      </c>
+      <c r="C15">
+        <v>11.15</v>
+      </c>
+      <c r="E15">
+        <v>257</v>
+      </c>
+      <c r="F15">
+        <v>2122.32</v>
+      </c>
+      <c r="G15">
+        <v>11.05</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>0.991432548840077</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="1"/>
+        <v>-0.0999999999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16">
+        <v>319</v>
+      </c>
+      <c r="B16">
+        <v>2132.51</v>
+      </c>
+      <c r="C16">
+        <v>11.11</v>
+      </c>
+      <c r="E16">
+        <v>319</v>
+      </c>
+      <c r="F16">
+        <v>2117.68</v>
+      </c>
+      <c r="G16">
+        <v>11.03</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="0"/>
+        <v>0.993045753595528</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="1"/>
+        <v>-0.0800000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17">
+        <v>320</v>
+      </c>
+      <c r="B17">
+        <v>1844.32</v>
+      </c>
+      <c r="C17">
+        <v>9.61</v>
+      </c>
+      <c r="E17">
+        <v>320</v>
+      </c>
+      <c r="F17">
+        <v>2030.39</v>
+      </c>
+      <c r="G17">
+        <v>10.57</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="0"/>
+        <v>1.10088813221133</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="1"/>
+        <v>0.960000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18">
+        <v>321</v>
+      </c>
+      <c r="B18">
+        <v>2137.09</v>
+      </c>
+      <c r="C18">
+        <v>11.13</v>
+      </c>
+      <c r="E18">
+        <v>321</v>
+      </c>
+      <c r="F18">
+        <v>2117.35</v>
+      </c>
+      <c r="G18">
+        <v>11.03</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="0"/>
+        <v>0.990763140532219</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="1"/>
+        <v>-0.100000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19">
+        <v>417</v>
+      </c>
+      <c r="B19">
+        <v>2128.93</v>
+      </c>
+      <c r="C19">
+        <v>11.09</v>
+      </c>
+      <c r="E19">
+        <v>417</v>
+      </c>
+      <c r="F19">
+        <v>2106.87</v>
+      </c>
+      <c r="G19">
+        <v>10.97</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="0"/>
+        <v>0.989637987157868</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="1"/>
+        <v>-0.119999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20">
+        <v>479</v>
+      </c>
+      <c r="B20">
+        <v>2122.75</v>
+      </c>
+      <c r="C20">
+        <v>11.06</v>
+      </c>
+      <c r="E20">
+        <v>479</v>
+      </c>
+      <c r="F20">
+        <v>2104.71</v>
+      </c>
+      <c r="G20">
+        <v>10.96</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="0"/>
+        <v>0.991501589918737</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="1"/>
+        <v>-0.0999999999999996</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21">
+        <v>480</v>
+      </c>
+      <c r="B21">
+        <v>2031.16</v>
+      </c>
+      <c r="C21">
+        <v>10.58</v>
+      </c>
+      <c r="E21">
+        <v>480</v>
+      </c>
+      <c r="F21">
+        <v>2030.49</v>
+      </c>
+      <c r="G21">
+        <v>10.58</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="0"/>
+        <v>0.999670139230784</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22">
+        <v>511</v>
+      </c>
+      <c r="B22">
+        <v>2128.31</v>
+      </c>
+      <c r="C22">
+        <v>11.08</v>
+      </c>
+      <c r="E22">
+        <v>511</v>
+      </c>
+      <c r="F22">
+        <v>2111.58</v>
+      </c>
+      <c r="G22">
+        <v>11</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="0"/>
+        <v>0.992139303015068</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="1"/>
+        <v>-0.0800000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23">
+        <v>512</v>
+      </c>
+      <c r="B23">
+        <v>962.479</v>
+      </c>
+      <c r="C23">
+        <v>5.01</v>
+      </c>
+      <c r="E23">
+        <v>512</v>
+      </c>
+      <c r="F23">
+        <v>954.884</v>
+      </c>
+      <c r="G23">
+        <v>4.97</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="0"/>
+        <v>0.992108918740045</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="1"/>
+        <v>-0.04</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24">
+        <v>639</v>
+      </c>
+      <c r="B24">
+        <v>2096.57</v>
+      </c>
+      <c r="C24">
+        <v>10.92</v>
+      </c>
+      <c r="E24">
+        <v>639</v>
+      </c>
+      <c r="F24">
+        <v>2096.74</v>
+      </c>
+      <c r="G24">
+        <v>10.92</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="0"/>
+        <v>1.00008108481949</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25">
+        <v>640</v>
+      </c>
+      <c r="B25">
+        <v>976.537</v>
+      </c>
+      <c r="C25">
+        <v>5.09</v>
+      </c>
+      <c r="E25">
+        <v>640</v>
+      </c>
+      <c r="F25">
+        <v>965.312</v>
+      </c>
+      <c r="G25">
+        <v>5.03</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="0"/>
+        <v>0.98850529985039</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="1"/>
+        <v>-0.0599999999999996</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26">
+        <v>767</v>
+      </c>
+      <c r="B26">
+        <v>2089.53</v>
+      </c>
+      <c r="C26">
+        <v>10.88</v>
+      </c>
+      <c r="E26">
+        <v>767</v>
+      </c>
+      <c r="F26">
+        <v>2096.22</v>
+      </c>
+      <c r="G26">
+        <v>10.92</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="0"/>
+        <v>1.00320167693213</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="1"/>
+        <v>0.0399999999999991</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27">
+        <v>768</v>
+      </c>
+      <c r="B27">
+        <v>975.947</v>
+      </c>
+      <c r="C27">
+        <v>5.08</v>
+      </c>
+      <c r="E27">
+        <v>768</v>
+      </c>
+      <c r="F27">
+        <v>966.518</v>
+      </c>
+      <c r="G27">
+        <v>5.03</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="0"/>
+        <v>0.990338614699364</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="1"/>
+        <v>-0.0499999999999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28">
+        <v>769</v>
+      </c>
+      <c r="B28">
+        <v>2089</v>
+      </c>
+      <c r="C28">
+        <v>10.88</v>
+      </c>
+      <c r="D28"/>
+      <c r="E28">
+        <v>769</v>
+      </c>
+      <c r="F28">
+        <v>2093.26</v>
+      </c>
+      <c r="G28">
+        <v>10.9</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="0"/>
+        <v>1.00203925323121</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="1"/>
+        <v>0.0199999999999996</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
   <drawing r:id="rId1"/>
+  <tableParts count="3">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>